<commit_message>
Final draft with TC ON
</commit_message>
<xml_diff>
--- a/Data_Tables2.xlsx
+++ b/Data_Tables2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-5355" yWindow="1620" windowWidth="15000" windowHeight="3690" tabRatio="713" activeTab="1"/>
+    <workbookView xWindow="-5355" yWindow="1620" windowWidth="15000" windowHeight="3690" tabRatio="713" firstSheet="2" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Species_breeds" sheetId="12" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="214">
   <si>
     <t xml:space="preserve">Species </t>
   </si>
@@ -249,9 +249,6 @@
     <t>Contract attributes</t>
   </si>
   <si>
-    <t xml:space="preserve">Number of levels </t>
-  </si>
-  <si>
     <t xml:space="preserve">Attribute levels </t>
   </si>
   <si>
@@ -273,15 +270,6 @@
     <t>Ovines = 5; 15; 25; 45 Lei / year</t>
   </si>
   <si>
-    <t xml:space="preserve">Application assistance only / independent agricultural advisor </t>
-  </si>
-  <si>
-    <t>5 / 10 years</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Individual / community </t>
-  </si>
-  <si>
     <t>Table 1: Attributes and attribute levels used in the CE</t>
   </si>
   <si>
@@ -652,6 +640,36 @@
   </si>
   <si>
     <t>The proportion of the farm animal population sampled accounted for by the most popular breed.</t>
+  </si>
+  <si>
+    <t>5 years / 10 years</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Basic assistance to complete the scheme application form 
+Additional advisory support throughout the scheme (e.g. additional training for animal breeding) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Individually managed  conservation scheme /programme
+Community managed conservation scheme programme
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No. of levels </t>
+  </si>
+  <si>
+    <t>Expected sign</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>Coding</t>
+  </si>
+  <si>
+    <t>Effects</t>
+  </si>
+  <si>
+    <t>Discrete</t>
   </si>
 </sst>
 </file>
@@ -863,7 +881,7 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1017,6 +1035,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1033,13 +1052,27 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1250,11 +1283,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="131764224"/>
-        <c:axId val="131765760"/>
+        <c:axId val="126114432"/>
+        <c:axId val="126148992"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="131764224"/>
+        <c:axId val="126114432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1264,7 +1297,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="131765760"/>
+        <c:crossAx val="126148992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1272,7 +1305,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="131765760"/>
+        <c:axId val="126148992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1283,7 +1316,7 @@
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="131764224"/>
+        <c:crossAx val="126114432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1389,11 +1422,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="141832192"/>
-        <c:axId val="141833728"/>
+        <c:axId val="127502208"/>
+        <c:axId val="127503744"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="141832192"/>
+        <c:axId val="127502208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1403,7 +1436,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141833728"/>
+        <c:crossAx val="127503744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1411,7 +1444,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="141833728"/>
+        <c:axId val="127503744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1422,13 +1455,14 @@
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141832192"/>
+        <c:crossAx val="127502208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1568,12 +1602,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="141883264"/>
-        <c:axId val="141884800"/>
+        <c:axId val="128000000"/>
+        <c:axId val="128001536"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="141883264"/>
+        <c:axId val="128000000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1582,7 +1616,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141884800"/>
+        <c:crossAx val="128001536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1590,7 +1624,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="141884800"/>
+        <c:axId val="128001536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1601,7 +1635,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141883264"/>
+        <c:crossAx val="128000000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1715,12 +1749,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="44881408"/>
-        <c:axId val="44882944"/>
+        <c:axId val="127403520"/>
+        <c:axId val="127405056"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="44881408"/>
+        <c:axId val="127403520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1729,7 +1763,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44882944"/>
+        <c:crossAx val="127405056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1737,7 +1771,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="44882944"/>
+        <c:axId val="127405056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1748,7 +1782,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44881408"/>
+        <c:crossAx val="127403520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2936,216 +2970,216 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="65" t="s">
+      <c r="A4" s="66" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="27">
         <v>34</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D4" s="28">
         <v>47</v>
       </c>
       <c r="E4" s="28" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="66"/>
+      <c r="A5" s="67"/>
       <c r="B5" s="4">
         <v>25</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D5" s="25">
         <v>31</v>
       </c>
       <c r="E5" s="25" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="65" t="s">
-        <v>97</v>
+      <c r="A6" s="66" t="s">
+        <v>93</v>
       </c>
       <c r="B6" s="27">
         <v>71</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D6" s="28">
         <v>56</v>
       </c>
       <c r="E6" s="28" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="66"/>
+      <c r="A7" s="67"/>
       <c r="B7" s="25">
         <v>18</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D7" s="25">
         <v>20</v>
       </c>
       <c r="E7" s="25" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="65" t="s">
-        <v>100</v>
+      <c r="A8" s="66" t="s">
+        <v>96</v>
       </c>
       <c r="B8" s="28">
         <v>46</v>
       </c>
       <c r="C8" s="27" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D8" s="28">
         <v>37</v>
       </c>
       <c r="E8" s="28" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="66"/>
+      <c r="A9" s="67"/>
       <c r="B9" s="25">
         <v>26</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D9" s="25">
         <v>19</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="65" t="s">
+      <c r="A10" s="66" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="27">
         <v>72</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D10" s="28">
         <v>83</v>
       </c>
       <c r="E10" s="28" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="66"/>
+      <c r="A11" s="67"/>
       <c r="B11" s="4">
         <v>11</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D11" s="25">
         <v>12</v>
       </c>
       <c r="E11" s="25" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="67" t="s">
+      <c r="A12" s="68" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="27">
         <v>57</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D12" s="28">
         <v>61</v>
       </c>
       <c r="E12" s="28" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="64"/>
+      <c r="A13" s="65"/>
       <c r="B13" s="4">
         <v>23</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D13" s="25">
         <v>28</v>
       </c>
       <c r="E13" s="25" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="63" t="s">
-        <v>109</v>
+      <c r="A14" s="64" t="s">
+        <v>105</v>
       </c>
       <c r="B14" s="5">
         <v>49</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D14" s="24">
         <v>51</v>
       </c>
       <c r="E14" s="24" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="64"/>
+      <c r="A15" s="65"/>
       <c r="B15" s="4">
         <v>16</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D15" s="25">
         <v>17</v>
       </c>
       <c r="E15" s="25" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -3179,139 +3213,139 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="40" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B3" s="40" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C3" s="40" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="41" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B4" s="41" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C4" s="42" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="41" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B5" s="41" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C5" s="42" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A6" s="41" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B6" s="41" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C6" s="42" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A7" s="41" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B7" s="41" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C7" s="42" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="41" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B8" s="41" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C8" s="42" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="41" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B9" s="41" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C9" s="42" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="41" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B10" s="41" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C10" s="42" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="41" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B11" s="41" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C11" s="42" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="41" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B12" s="41" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C12" s="42" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="43" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B13" s="43" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C13" s="44" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A14" s="45" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B14" s="45" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C14" s="46" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -3328,7 +3362,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3342,36 +3376,36 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B1" s="23"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="47" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B3" s="47" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C3" s="48" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D3" s="48" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="E3" s="48" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="F3" s="61" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="49" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B4" s="49" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C4" s="50">
         <v>0.83</v>
@@ -3383,15 +3417,15 @@
         <v>0.49</v>
       </c>
       <c r="F4" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="49" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B5" s="49" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C5" s="50">
         <v>4.2300000000000004</v>
@@ -3400,18 +3434,18 @@
         <v>1.44</v>
       </c>
       <c r="E5" s="42" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="F5" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A6" s="49" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B6" s="49" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C6" s="50">
         <v>1.58</v>
@@ -3420,18 +3454,18 @@
         <v>0.61</v>
       </c>
       <c r="E6" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="F6" t="s">
         <v>164</v>
-      </c>
-      <c r="F6" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A7" s="49" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B7" s="49" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C7" s="51">
         <v>3.8</v>
@@ -3443,18 +3477,18 @@
         <v>566</v>
       </c>
       <c r="F7" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="G7" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="52" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B8" s="52" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C8" s="50">
         <v>2.59</v>
@@ -3463,18 +3497,18 @@
         <v>1.05</v>
       </c>
       <c r="E8" s="49" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="F8" s="39" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="52" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B9" s="52" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C9" s="50">
         <v>0.4</v>
@@ -3488,10 +3522,10 @@
     </row>
     <row r="10" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A10" s="52" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B10" s="52" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C10" s="50">
         <v>0.89</v>
@@ -3505,10 +3539,10 @@
     </row>
     <row r="11" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A11" s="52" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B11" s="52" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C11" s="50">
         <v>0.32</v>
@@ -3522,10 +3556,10 @@
     </row>
     <row r="12" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A12" s="52" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B12" s="52" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C12" s="50">
         <v>0.21</v>
@@ -3539,10 +3573,10 @@
     </row>
     <row r="13" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A13" s="52" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B13" s="52" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C13" s="50">
         <v>1.39</v>
@@ -3556,10 +3590,10 @@
     </row>
     <row r="14" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A14" s="53" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B14" s="53" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C14" s="54">
         <v>0.08</v>
@@ -3573,10 +3607,10 @@
     </row>
     <row r="15" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A15" s="55" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B15" s="55" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C15" s="56">
         <v>0.47</v>
@@ -3656,23 +3690,23 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B3" s="23" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B5">
         <v>3368</v>
@@ -3683,7 +3717,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B6">
         <v>352</v>
@@ -3694,7 +3728,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B7">
         <v>49</v>
@@ -3705,7 +3739,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B8">
         <v>388</v>
@@ -3716,7 +3750,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B9">
         <v>166</v>
@@ -3730,7 +3764,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B10">
         <v>1261</v>
@@ -3744,7 +3778,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B11">
         <v>565</v>
@@ -3758,7 +3792,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B12">
         <f>SUM(B6:B10)</f>
@@ -3775,7 +3809,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B13">
         <f>SUM(B6:B9)</f>
@@ -3792,7 +3826,7 @@
     </row>
     <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="23" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B14" s="58">
         <f>B13/B12*100</f>
@@ -3815,16 +3849,16 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B16" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D16" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -3837,7 +3871,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
@@ -3851,8 +3885,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="70" t="s">
-        <v>206</v>
+      <c r="A1" s="63" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
@@ -3860,16 +3894,16 @@
         <v>0</v>
       </c>
       <c r="B3" s="62" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C3" s="62" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="D3" s="62" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="E3" s="62" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -3883,7 +3917,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="E4" s="15">
         <v>39</v>
@@ -3900,7 +3934,7 @@
         <v>4</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="E5" s="15">
         <v>11</v>
@@ -3917,7 +3951,7 @@
         <v>13</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="E6" s="15" t="s">
         <v>7</v>
@@ -3934,7 +3968,7 @@
         <v>3</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="E7" s="15">
         <v>14</v>
@@ -3951,7 +3985,7 @@
         <v>9</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="E8" s="15">
         <v>52</v>
@@ -3968,20 +4002,20 @@
         <v>8</v>
       </c>
       <c r="D9" s="57" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="E9" s="57">
         <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="71" t="s">
-        <v>208</v>
-      </c>
-      <c r="B10" s="71"/>
-      <c r="C10" s="71"/>
-      <c r="D10" s="71"/>
-      <c r="E10" s="71"/>
+      <c r="A10" s="69" t="s">
+        <v>204</v>
+      </c>
+      <c r="B10" s="69"/>
+      <c r="C10" s="69"/>
+      <c r="D10" s="69"/>
+      <c r="E10" s="69"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="5"/>
@@ -4046,7 +4080,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B4" s="3">
         <v>81</v>
@@ -4285,7 +4319,7 @@
   <dimension ref="A1:P40"/>
   <sheetViews>
     <sheetView topLeftCell="A22" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+      <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4340,7 +4374,7 @@
       </c>
       <c r="G2" s="10"/>
       <c r="H2" s="10" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="I2" s="10">
         <v>5.2181818181818178</v>
@@ -4388,7 +4422,7 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="H3" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="I3">
         <v>2.7818181818181822</v>
@@ -4457,7 +4491,7 @@
         <v>4.21</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="I5" s="7">
         <v>5.2335329341317367</v>
@@ -4505,7 +4539,7 @@
         <v>4.08</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="I6" s="32">
         <f>8-I5</f>
@@ -4561,28 +4595,28 @@
         <v>2.2200000000000002</v>
       </c>
       <c r="H7" s="33" t="s">
+        <v>113</v>
+      </c>
+      <c r="I7" s="33" t="s">
+        <v>114</v>
+      </c>
+      <c r="J7" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="K7" s="33" t="s">
+        <v>116</v>
+      </c>
+      <c r="L7" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="I7" s="33" t="s">
+      <c r="M7" s="33" t="s">
         <v>118</v>
       </c>
-      <c r="J7" s="33" t="s">
+      <c r="N7" s="33" t="s">
         <v>119</v>
       </c>
-      <c r="K7" s="33" t="s">
+      <c r="O7" s="33" t="s">
         <v>120</v>
-      </c>
-      <c r="L7" s="33" t="s">
-        <v>121</v>
-      </c>
-      <c r="M7" s="33" t="s">
-        <v>122</v>
-      </c>
-      <c r="N7" s="33" t="s">
-        <v>123</v>
-      </c>
-      <c r="O7" s="33" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
@@ -4793,22 +4827,22 @@
         <v>17</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D2" s="20" t="s">
         <v>19</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F2" s="20" t="s">
         <v>21</v>
       </c>
       <c r="G2" s="20" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="H2" s="20" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -4864,16 +4898,16 @@
   <sheetData>
     <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C2" s="22" t="s">
         <v>20</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E2" s="22" t="s">
         <v>29</v>
@@ -5048,83 +5082,119 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.625" customWidth="1"/>
+    <col min="1" max="1" width="15.375" customWidth="1"/>
+    <col min="2" max="2" width="9.375" customWidth="1"/>
+    <col min="3" max="3" width="8.625" customWidth="1"/>
+    <col min="4" max="4" width="35.375" customWidth="1"/>
+    <col min="5" max="5" width="7.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="47" t="s">
         <v>73</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="48" t="s">
+        <v>208</v>
+      </c>
+      <c r="C3" s="48" t="s">
+        <v>211</v>
+      </c>
+      <c r="D3" s="47" t="s">
         <v>74</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="E3" s="48" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="50" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="15" t="s">
+      <c r="B4" s="50">
+        <v>2</v>
+      </c>
+      <c r="C4" s="74" t="s">
+        <v>212</v>
+      </c>
+      <c r="D4" s="49" t="s">
+        <v>205</v>
+      </c>
+      <c r="E4" s="50" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="50" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" s="50">
+        <v>2</v>
+      </c>
+      <c r="C5" s="74" t="s">
+        <v>212</v>
+      </c>
+      <c r="D5" s="49" t="s">
+        <v>206</v>
+      </c>
+      <c r="E5" s="50" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="50" t="s">
         <v>76</v>
       </c>
-      <c r="B4" s="15">
+      <c r="B6" s="50">
         <v>2</v>
       </c>
-      <c r="C4" s="15" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="15" t="s">
+      <c r="C6" s="74" t="s">
+        <v>212</v>
+      </c>
+      <c r="D6" s="49" t="s">
+        <v>207</v>
+      </c>
+      <c r="E6" s="50" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="69" t="s">
         <v>78</v>
       </c>
-      <c r="B5" s="15">
-        <v>2</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="B6" s="15">
-        <v>2</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="68" t="s">
+      <c r="B7" s="69">
+        <v>4</v>
+      </c>
+      <c r="C7" s="75" t="s">
+        <v>213</v>
+      </c>
+      <c r="D7" s="73" t="s">
         <v>79</v>
       </c>
-      <c r="B7" s="68">
-        <v>4</v>
-      </c>
-      <c r="C7" s="17" t="s">
+      <c r="E7" s="69" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="72"/>
+      <c r="B8" s="72"/>
+      <c r="C8" s="76" t="s">
+        <v>213</v>
+      </c>
+      <c r="D8" s="56" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="69"/>
-      <c r="B8" s="69"/>
-      <c r="C8" s="16" t="s">
-        <v>81</v>
-      </c>
+      <c r="E8" s="72"/>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B32" s="14"/>
@@ -5159,29 +5229,30 @@
       <c r="L35" s="15"/>
     </row>
     <row r="36" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B36" s="68"/>
-      <c r="C36" s="68"/>
+      <c r="B36" s="70"/>
+      <c r="C36" s="70"/>
       <c r="D36" s="17"/>
-      <c r="J36" s="68"/>
-      <c r="K36" s="68"/>
+      <c r="J36" s="70"/>
+      <c r="K36" s="70"/>
       <c r="L36" s="17"/>
     </row>
     <row r="37" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B37" s="69"/>
-      <c r="C37" s="69"/>
+      <c r="B37" s="71"/>
+      <c r="C37" s="71"/>
       <c r="D37" s="16"/>
-      <c r="J37" s="69"/>
-      <c r="K37" s="69"/>
+      <c r="J37" s="71"/>
+      <c r="K37" s="71"/>
       <c r="L37" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="J36:J37"/>
     <mergeCell ref="K36:K37"/>
     <mergeCell ref="B36:B37"/>
     <mergeCell ref="C36:C37"/>
+    <mergeCell ref="E7:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>